<commit_message>
Creating, changing downloads, uploads folder inside project for more convenient
</commit_message>
<xml_diff>
--- a/dataTestCase_Login.xlsx
+++ b/dataTestCase_Login.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>Search</t>
   </si>
@@ -118,6 +118,48 @@
   </si>
   <si>
     <t>Login with empty username and filled password</t>
+  </si>
+  <si>
+    <t>Login with both empty username and password</t>
+  </si>
+  <si>
+    <t>Login with invalid username and invalid password with more than 50 characters</t>
+  </si>
+  <si>
+    <t>andadahhashdnansasasdnaandadahhashdnansasasdnaandadahhashdnansasasdnaandadahhashdnansasasdnaandadahhashdnansasasdnaandadahhashdnansasasdnaandadahhashdnansasasdnaandadahhashdnansasasdna</t>
+  </si>
+  <si>
+    <t>Login with valid username and invalid password with more than 50 characters</t>
+  </si>
+  <si>
+    <t>jglnadsnandnasndkanjdnaskndajglnadsnandnasndkanjdnaskndajglnadsnandnasndkanjdnaskndajglnadsnandnasndkanjdnaskndajglnadsnandnasndkanjdnaskndajglnadsnandnasndkanjdnaskndajglnadsnandnasndkanjdnasknda</t>
+  </si>
+  <si>
+    <t>Login_invalidName_ValidPassword</t>
+  </si>
+  <si>
+    <t>Login with invalid username with more than 51 characters and valid password</t>
+  </si>
+  <si>
+    <t>isajdilalnflndnkjakdsbnkasbdkabsdkasjnisajdilalnflndnkjakdsbnkasbdkabsdkasjnisajdilalnflndnkjakdsbnkasbdkabsdkasjnisajdilalnflndnkjakdsbnkasbdkabsdkasjnisajdilalnflndnkjakdsbnkasbdkabsdkasjnisajdilalnflndnkjakdsbnkasbdkabsdkasjn</t>
+  </si>
+  <si>
+    <t>Login_EmptyName_InvalidPassword</t>
+  </si>
+  <si>
+    <t>Login with empty username and invalid password with more than 50 characters</t>
+  </si>
+  <si>
+    <t>pla,lmmwqinqndkalsdlkamaskdmakmckamkadknapla,lmmwqinqndkalsdlkamaskdmakmckamkadknapla,lmmwqinqndkalsdlkamaskdmakmckamkadknapla,lmmwqinqndkalsdlkamaskdmakmckamkadknapla,lmmwqinqndkalsdlkamaskdmakmckamkadkna</t>
+  </si>
+  <si>
+    <t>Login_InvalidName_EmptyPassword</t>
+  </si>
+  <si>
+    <t>Login with empty invalid username with more than 51 characters and empty password</t>
+  </si>
+  <si>
+    <t>jnjknasdankamckmawjnqwdnoqmomaskmdajnjknasdankamckmawjnqwdnoqmomaskmdajnjknasdankamckmawjnqwdnoqmomaskmdajnjknasdankamckmawjnqwdnoqmomaskmdajnjknasdankamckmawjnqwdnoqmomaskmdajnjknasdankamckmawjnqwdnoqmomaskmdajnjknasdankamckmawjnqwdnoqmomaskmdajnjknasdankamckmawjnqwdnoqmomaskmda</t>
   </si>
 </sst>
 </file>
@@ -126,9 +168,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -151,16 +193,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,28 +237,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -218,16 +261,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,7 +285,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,6 +299,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,28 +335,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -315,187 +357,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,6 +603,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -579,38 +645,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,6 +675,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -649,19 +700,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -679,7 +721,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -688,31 +730,31 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -721,92 +763,92 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,6 +870,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,13 +1274,13 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="40.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="2" max="2" width="77" customWidth="1"/>
     <col min="3" max="3" width="34.4380952380952" customWidth="1"/>
     <col min="4" max="5" width="17.5714285714286" customWidth="1"/>
     <col min="6" max="6" width="52.4285714285714" customWidth="1"/>
@@ -1412,68 +1458,130 @@
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:7">
+      <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:7">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="F12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" ht="13" customHeight="1" spans="1:7">
+      <c r="A13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="E13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:7">
+      <c r="A14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="6"/>

</xml_diff>